<commit_message>
new books are loaded
</commit_message>
<xml_diff>
--- a/BOOKS/no starch press/BOOKS.xlsx
+++ b/BOOKS/no starch press/BOOKS.xlsx
@@ -12,12 +12,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$38</definedName>
   </definedNames>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="107">
   <si>
     <t>NAME</t>
   </si>
@@ -324,9 +324,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">The Big Book of Small </t>
-  </si>
-  <si>
     <t xml:space="preserve">Python Projects
 81 Easy Practice Programs
 </t>
@@ -383,13 +380,30 @@
   </si>
   <si>
     <t>Adam Schroeder,                                                                  Christian Mayer, and                                                                              Ann Marie Ward</t>
+  </si>
+  <si>
+    <t>PRICE USD</t>
+  </si>
+  <si>
+    <t>PRICE INR</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>The Big Book of Small Python Projects</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="165" formatCode="_ [$₹-4009]\ * #,##0.00_ ;_ [$₹-4009]\ * \-#,##0.00_ ;_ [$₹-4009]\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="166" formatCode="&quot;₹&quot;\ #,##0.00"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -404,6 +418,28 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Arial Black"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -420,7 +456,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -519,21 +555,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -628,11 +649,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -668,35 +714,85 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -3027,35 +3123,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P38"/>
+  <dimension ref="A1:P39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="31.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" style="1" customWidth="1"/>
-    <col min="2" max="2" width="49" style="3" customWidth="1"/>
+    <col min="2" max="2" width="57" style="38" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="25.85546875" style="23" customWidth="1"/>
+    <col min="6" max="6" width="30.140625" style="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="4" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E1"/>
-      <c r="F1"/>
+      <c r="E1" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>104</v>
+      </c>
       <c r="G1"/>
       <c r="H1"/>
       <c r="I1"/>
@@ -3065,20 +3167,27 @@
       <c r="P1"/>
     </row>
     <row r="2" spans="1:16" ht="99.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="20"/>
-      <c r="B2" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="C2" s="14" t="s">
+      <c r="A2" s="19"/>
+      <c r="B2" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="15" t="s">
-        <v>102</v>
+      <c r="D2" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="E2" s="21">
+        <v>39.99</v>
+      </c>
+      <c r="F2" s="26">
+        <f>E2*83.19</f>
+        <v>3326.7681000000002</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
-      <c r="B3" s="22" t="s">
+      <c r="A3" s="18"/>
+      <c r="B3" s="34" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="5" t="s">
@@ -3086,23 +3195,37 @@
       </c>
       <c r="D3" s="8" t="s">
         <v>3</v>
+      </c>
+      <c r="E3" s="22">
+        <v>34.950000000000003</v>
+      </c>
+      <c r="F3" s="26">
+        <f>E3*83.19</f>
+        <v>2907.4905000000003</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4"/>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="34" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
+      </c>
+      <c r="E4" s="22">
+        <v>44.99</v>
+      </c>
+      <c r="F4" s="26">
+        <f t="shared" ref="F4:F39" si="0">E4*83.19</f>
+        <v>3742.7181</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="34" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="5" t="s">
@@ -3110,69 +3233,111 @@
       </c>
       <c r="D5" s="8" t="s">
         <v>5</v>
+      </c>
+      <c r="E5" s="22">
+        <v>29.95</v>
+      </c>
+      <c r="F5" s="26">
+        <f t="shared" si="0"/>
+        <v>2491.5405000000001</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6"/>
-      <c r="B6" s="5" t="s">
-        <v>94</v>
+      <c r="B6" s="34" t="s">
+        <v>93</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
+      </c>
+      <c r="E6" s="22">
+        <v>59.99</v>
+      </c>
+      <c r="F6" s="26">
+        <f t="shared" si="0"/>
+        <v>4990.5681000000004</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
-      <c r="B7" s="22" t="s">
-        <v>96</v>
+      <c r="B7" s="34" t="s">
+        <v>95</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
+      </c>
+      <c r="E7" s="22">
+        <v>39.950000000000003</v>
+      </c>
+      <c r="F7" s="26">
+        <f t="shared" si="0"/>
+        <v>3323.4405000000002</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
-      <c r="B8" s="5" t="s">
-        <v>98</v>
+      <c r="B8" s="34" t="s">
+        <v>97</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
+      </c>
+      <c r="E8" s="22">
+        <v>39.99</v>
+      </c>
+      <c r="F8" s="26">
+        <f t="shared" si="0"/>
+        <v>3326.7681000000002</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
-      <c r="B9" s="5" t="s">
-        <v>100</v>
+      <c r="B9" s="34" t="s">
+        <v>99</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
+      </c>
+      <c r="E9" s="22">
+        <v>29.99</v>
+      </c>
+      <c r="F9" s="26">
+        <f t="shared" si="0"/>
+        <v>2494.8680999999997</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="35" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D10" s="10"/>
+      <c r="E10" s="22">
+        <v>49.99</v>
+      </c>
+      <c r="F10" s="26">
+        <f t="shared" si="0"/>
+        <v>4158.6680999999999</v>
+      </c>
     </row>
     <row r="11" spans="1:16" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="34" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="5" t="s">
@@ -3180,11 +3345,18 @@
       </c>
       <c r="D11" s="8" t="s">
         <v>18</v>
+      </c>
+      <c r="E11" s="22">
+        <v>39.950000000000003</v>
+      </c>
+      <c r="F11" s="26">
+        <f t="shared" si="0"/>
+        <v>3323.4405000000002</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="34" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="5" t="s">
@@ -3192,11 +3364,18 @@
       </c>
       <c r="D12" s="8" t="s">
         <v>21</v>
+      </c>
+      <c r="E12" s="22">
+        <v>59.99</v>
+      </c>
+      <c r="F12" s="26">
+        <f t="shared" si="0"/>
+        <v>4990.5681000000004</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="34" t="s">
         <v>23</v>
       </c>
       <c r="C13" s="5" t="s">
@@ -3204,11 +3383,18 @@
       </c>
       <c r="D13" s="8" t="s">
         <v>24</v>
+      </c>
+      <c r="E13" s="22">
+        <v>29.95</v>
+      </c>
+      <c r="F13" s="26">
+        <f t="shared" si="0"/>
+        <v>2491.5405000000001</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="34" t="s">
         <v>25</v>
       </c>
       <c r="C14" s="5" t="s">
@@ -3216,11 +3402,18 @@
       </c>
       <c r="D14" s="8" t="s">
         <v>26</v>
+      </c>
+      <c r="E14" s="22">
+        <v>29.99</v>
+      </c>
+      <c r="F14" s="26">
+        <f t="shared" si="0"/>
+        <v>2494.8680999999997</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="34" t="s">
         <v>28</v>
       </c>
       <c r="C15" s="5" t="s">
@@ -3228,11 +3421,18 @@
       </c>
       <c r="D15" s="8" t="s">
         <v>29</v>
+      </c>
+      <c r="E15" s="22">
+        <v>34.99</v>
+      </c>
+      <c r="F15" s="26">
+        <f t="shared" si="0"/>
+        <v>2910.8181</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="35" t="s">
         <v>31</v>
       </c>
       <c r="C16" s="5" t="s">
@@ -3241,10 +3441,17 @@
       <c r="D16" s="8" t="s">
         <v>32</v>
       </c>
+      <c r="E16" s="22">
+        <v>29.95</v>
+      </c>
+      <c r="F16" s="26">
+        <f t="shared" si="0"/>
+        <v>2491.5405000000001</v>
+      </c>
     </row>
-    <row r="17" spans="1:4" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="34" t="s">
         <v>34</v>
       </c>
       <c r="C17" s="5" t="s">
@@ -3253,10 +3460,17 @@
       <c r="D17" s="8" t="s">
         <v>35</v>
       </c>
+      <c r="E17" s="22">
+        <v>39.99</v>
+      </c>
+      <c r="F17" s="26">
+        <f t="shared" si="0"/>
+        <v>3326.7681000000002</v>
+      </c>
     </row>
-    <row r="18" spans="1:4" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="34" t="s">
         <v>37</v>
       </c>
       <c r="C18" s="5" t="s">
@@ -3265,10 +3479,17 @@
       <c r="D18" s="8" t="s">
         <v>38</v>
       </c>
+      <c r="E18" s="22">
+        <v>49.99</v>
+      </c>
+      <c r="F18" s="26">
+        <f t="shared" si="0"/>
+        <v>4158.6680999999999</v>
+      </c>
     </row>
-    <row r="19" spans="1:4" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="36" t="s">
         <v>40</v>
       </c>
       <c r="C19" s="5" t="s">
@@ -3277,10 +3498,17 @@
       <c r="D19" s="8" t="s">
         <v>41</v>
       </c>
+      <c r="E19" s="22">
+        <v>29.99</v>
+      </c>
+      <c r="F19" s="26">
+        <f t="shared" si="0"/>
+        <v>2494.8680999999997</v>
+      </c>
     </row>
-    <row r="20" spans="1:4" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="34" t="s">
         <v>43</v>
       </c>
       <c r="C20" s="5" t="s">
@@ -3289,10 +3517,17 @@
       <c r="D20" s="8" t="s">
         <v>44</v>
       </c>
+      <c r="E20" s="22">
+        <v>29.99</v>
+      </c>
+      <c r="F20" s="26">
+        <f t="shared" si="0"/>
+        <v>2494.8680999999997</v>
+      </c>
     </row>
-    <row r="21" spans="1:4" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="35" t="s">
         <v>46</v>
       </c>
       <c r="C21" s="5" t="s">
@@ -3301,10 +3536,17 @@
       <c r="D21" s="8" t="s">
         <v>47</v>
       </c>
+      <c r="E21" s="22">
+        <v>39.99</v>
+      </c>
+      <c r="F21" s="26">
+        <f t="shared" si="0"/>
+        <v>3326.7681000000002</v>
+      </c>
     </row>
-    <row r="22" spans="1:4" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="35" t="s">
         <v>48</v>
       </c>
       <c r="C22" s="5" t="s">
@@ -3313,10 +3555,17 @@
       <c r="D22" s="8" t="s">
         <v>49</v>
       </c>
+      <c r="E22" s="22">
+        <v>39.950000000000003</v>
+      </c>
+      <c r="F22" s="26">
+        <f t="shared" si="0"/>
+        <v>3323.4405000000002</v>
+      </c>
     </row>
-    <row r="23" spans="1:4" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="34" t="s">
         <v>52</v>
       </c>
       <c r="C23" s="5" t="s">
@@ -3325,10 +3574,17 @@
       <c r="D23" s="8" t="s">
         <v>51</v>
       </c>
+      <c r="E23" s="22">
+        <v>44.99</v>
+      </c>
+      <c r="F23" s="26">
+        <f t="shared" si="0"/>
+        <v>3742.7181</v>
+      </c>
     </row>
-    <row r="24" spans="1:4" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="35" t="s">
         <v>54</v>
       </c>
       <c r="C24" s="5" t="s">
@@ -3337,10 +3593,17 @@
       <c r="D24" s="8" t="s">
         <v>55</v>
       </c>
+      <c r="E24" s="22">
+        <v>59.95</v>
+      </c>
+      <c r="F24" s="26">
+        <f t="shared" si="0"/>
+        <v>4987.2404999999999</v>
+      </c>
     </row>
-    <row r="25" spans="1:4" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
-      <c r="B25" s="22" t="s">
+      <c r="B25" s="34" t="s">
         <v>57</v>
       </c>
       <c r="C25" s="5" t="s">
@@ -3349,10 +3612,17 @@
       <c r="D25" s="8" t="s">
         <v>58</v>
       </c>
+      <c r="E25" s="22">
+        <v>44.99</v>
+      </c>
+      <c r="F25" s="26">
+        <f t="shared" si="0"/>
+        <v>3742.7181</v>
+      </c>
     </row>
-    <row r="26" spans="1:4" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="34" t="s">
         <v>59</v>
       </c>
       <c r="C26" s="5" t="s">
@@ -3361,10 +3631,17 @@
       <c r="D26" s="8" t="s">
         <v>60</v>
       </c>
+      <c r="E26" s="22">
+        <v>27.95</v>
+      </c>
+      <c r="F26" s="26">
+        <f t="shared" si="0"/>
+        <v>2325.1605</v>
+      </c>
     </row>
-    <row r="27" spans="1:4" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="39" t="s">
         <v>63</v>
       </c>
       <c r="C27" s="5" t="s">
@@ -3373,10 +3650,17 @@
       <c r="D27" s="8" t="s">
         <v>64</v>
       </c>
+      <c r="E27" s="22">
+        <v>29.99</v>
+      </c>
+      <c r="F27" s="26">
+        <f t="shared" si="0"/>
+        <v>2494.8680999999997</v>
+      </c>
     </row>
-    <row r="28" spans="1:4" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="34" t="s">
         <v>65</v>
       </c>
       <c r="C28" s="5" t="s">
@@ -3385,10 +3669,17 @@
       <c r="D28" s="8" t="s">
         <v>67</v>
       </c>
+      <c r="E28" s="22">
+        <v>34.99</v>
+      </c>
+      <c r="F28" s="26">
+        <f t="shared" si="0"/>
+        <v>2910.8181</v>
+      </c>
     </row>
-    <row r="29" spans="1:4" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9"/>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="34" t="s">
         <v>68</v>
       </c>
       <c r="C29" s="5" t="s">
@@ -3397,10 +3688,17 @@
       <c r="D29" s="8" t="s">
         <v>69</v>
       </c>
+      <c r="E29" s="22">
+        <v>39.950000000000003</v>
+      </c>
+      <c r="F29" s="26">
+        <f t="shared" si="0"/>
+        <v>3323.4405000000002</v>
+      </c>
     </row>
-    <row r="30" spans="1:4" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="9"/>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="34" t="s">
         <v>71</v>
       </c>
       <c r="C30" s="5" t="s">
@@ -3409,10 +3707,17 @@
       <c r="D30" s="8" t="s">
         <v>72</v>
       </c>
+      <c r="E30" s="22">
+        <v>44.99</v>
+      </c>
+      <c r="F30" s="26">
+        <f t="shared" si="0"/>
+        <v>3742.7181</v>
+      </c>
     </row>
-    <row r="31" spans="1:4" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="9"/>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="35" t="s">
         <v>73</v>
       </c>
       <c r="C31" s="5" t="s">
@@ -3421,10 +3726,17 @@
       <c r="D31" s="8" t="s">
         <v>74</v>
       </c>
+      <c r="E31" s="22">
+        <v>49.99</v>
+      </c>
+      <c r="F31" s="26">
+        <f t="shared" si="0"/>
+        <v>4158.6680999999999</v>
+      </c>
     </row>
-    <row r="32" spans="1:4" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="9"/>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="34" t="s">
         <v>76</v>
       </c>
       <c r="C32" s="5" t="s">
@@ -3433,10 +3745,17 @@
       <c r="D32" s="8" t="s">
         <v>77</v>
       </c>
+      <c r="E32" s="22">
+        <v>34.950000000000003</v>
+      </c>
+      <c r="F32" s="26">
+        <f t="shared" si="0"/>
+        <v>2907.4905000000003</v>
+      </c>
     </row>
-    <row r="33" spans="1:4" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="9"/>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="34" t="s">
         <v>78</v>
       </c>
       <c r="C33" s="5" t="s">
@@ -3445,10 +3764,17 @@
       <c r="D33" s="8" t="s">
         <v>79</v>
       </c>
+      <c r="E33" s="22">
+        <v>34.950000000000003</v>
+      </c>
+      <c r="F33" s="26">
+        <f t="shared" si="0"/>
+        <v>2907.4905000000003</v>
+      </c>
     </row>
-    <row r="34" spans="1:4" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="9"/>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="34" t="s">
         <v>81</v>
       </c>
       <c r="C34" s="5" t="s">
@@ -3457,10 +3783,17 @@
       <c r="D34" s="8" t="s">
         <v>82</v>
       </c>
+      <c r="E34" s="22">
+        <v>29.95</v>
+      </c>
+      <c r="F34" s="26">
+        <f t="shared" si="0"/>
+        <v>2491.5405000000001</v>
+      </c>
     </row>
-    <row r="35" spans="1:4" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="9"/>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="35" t="s">
         <v>84</v>
       </c>
       <c r="C35" s="5" t="s">
@@ -3469,41 +3802,82 @@
       <c r="D35" s="8" t="s">
         <v>85</v>
       </c>
+      <c r="E35" s="22">
+        <v>29.99</v>
+      </c>
+      <c r="F35" s="26">
+        <f t="shared" si="0"/>
+        <v>2494.8680999999997</v>
+      </c>
     </row>
-    <row r="36" spans="1:4" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="9"/>
-      <c r="B36" s="5" t="s">
-        <v>86</v>
+      <c r="B36" s="34" t="s">
+        <v>106</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D36" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="E36" s="22">
+        <v>39.99</v>
+      </c>
+      <c r="F36" s="26">
+        <f t="shared" si="0"/>
+        <v>3326.7681000000002</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="9"/>
+      <c r="B37" s="34" t="s">
         <v>87</v>
       </c>
+      <c r="C37" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="E37" s="22">
+        <v>34.99</v>
+      </c>
+      <c r="F37" s="26">
+        <f t="shared" si="0"/>
+        <v>2910.8181</v>
+      </c>
     </row>
-    <row r="37" spans="1:4" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="9"/>
-      <c r="B37" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="D37" s="8" t="s">
+    <row r="38" spans="1:6" ht="99.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="11"/>
+      <c r="B38" s="37" t="s">
         <v>89</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="99.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="11"/>
-      <c r="B38" s="12" t="s">
-        <v>90</v>
       </c>
       <c r="C38" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D38" s="13" t="s">
-        <v>91</v>
+      <c r="D38" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E38" s="28">
+        <v>39.99</v>
+      </c>
+      <c r="F38" s="29">
+        <f t="shared" si="0"/>
+        <v>3326.7681000000002</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="84" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D39" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="E39" s="32">
+        <f>SUM(E2:E38)</f>
+        <v>1447.1100000000004</v>
+      </c>
+      <c r="F39" s="30">
+        <f t="shared" si="0"/>
+        <v>120385.08090000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>